<commit_message>
v 4.2.2 modifications to renal + add rep hfh
</commit_message>
<xml_diff>
--- a/metadata/meta_variables.xlsx
+++ b/metadata/meta_variables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\STATISTIK\Projects\20210525_shfdb4\dm\metadata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\STATISTIK\Projects\20210525_shfdb4\dm\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79713D2B-9F66-4690-AB58-F958808E234A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2457C06C-F752-43E2-8931-D97EC0361683}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4035" yWindow="4320" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="486">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="489">
   <si>
     <t>lopnr</t>
   </si>
@@ -964,9 +964,6 @@
     <t>Follow-up referral speciality</t>
   </si>
   <si>
-    <t>QoL EQ-5D</t>
-  </si>
-  <si>
     <t>BMI</t>
   </si>
   <si>
@@ -1228,12 +1225,6 @@
     <t>Renal failure</t>
   </si>
   <si>
-    <t>Renal failure hospitalization</t>
-  </si>
-  <si>
-    <t>sos_out_hosprenal</t>
-  </si>
-  <si>
     <t>sos_com_respiratory</t>
   </si>
   <si>
@@ -1345,9 +1336,6 @@
     <t>2008-02-01-</t>
   </si>
   <si>
-    <t>sos_outtime_hosprenal</t>
-  </si>
-  <si>
     <t>shf_bpdia_dis</t>
   </si>
   <si>
@@ -1478,6 +1466,27 @@
   </si>
   <si>
     <t>Charlson Comorbidity Index age-adjusted</t>
+  </si>
+  <si>
+    <t>EQ5D-vas</t>
+  </si>
+  <si>
+    <t>sos_out_hosprenalacute</t>
+  </si>
+  <si>
+    <t>sos_outtime_hosprenalacute</t>
+  </si>
+  <si>
+    <t>Acute renal failure hospitalization</t>
+  </si>
+  <si>
+    <t>sos_out_renalendstage</t>
+  </si>
+  <si>
+    <t>sos_outtime_renalendstage</t>
+  </si>
+  <si>
+    <t>End-stage renal failure</t>
   </si>
 </sst>
 </file>
@@ -1540,7 +1549,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1549,6 +1558,10 @@
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1847,10 +1860,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E226"/>
+  <dimension ref="A1:E228"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A150" workbookViewId="0">
-      <selection activeCell="D174" sqref="D174"/>
+    <sheetView tabSelected="1" topLeftCell="A184" workbookViewId="0">
+      <selection activeCell="B188" sqref="B188"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1891,23 +1904,23 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="E4" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="E5" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1953,7 +1966,7 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="E10" t="s">
         <v>201</v>
@@ -2112,7 +2125,7 @@
         <v>19</v>
       </c>
       <c r="B25" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -2123,7 +2136,7 @@
         <v>221</v>
       </c>
       <c r="C26" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>222</v>
@@ -2164,7 +2177,7 @@
         <v>23</v>
       </c>
       <c r="B30" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>204</v>
@@ -2181,15 +2194,15 @@
         <v>228</v>
       </c>
       <c r="E31" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="B32" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="C32" t="s">
         <v>228</v>
@@ -2200,10 +2213,10 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="B33" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="C33" t="s">
         <v>228</v>
@@ -2237,15 +2250,15 @@
         <v>233</v>
       </c>
       <c r="E35" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="B36" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="C36" t="s">
         <v>233</v>
@@ -2256,10 +2269,10 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="B37" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="C37" t="s">
         <v>233</v>
@@ -2279,15 +2292,15 @@
         <v>233</v>
       </c>
       <c r="E38" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="B39" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="C39" t="s">
         <v>233</v>
@@ -2298,10 +2311,10 @@
     </row>
     <row r="40" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="B40" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="C40" t="s">
         <v>233</v>
@@ -2343,7 +2356,7 @@
         <v>237</v>
       </c>
       <c r="E43" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -2359,10 +2372,10 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="B45" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="C45" t="s">
         <v>237</v>
@@ -2373,10 +2386,10 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="B46" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="C46" t="s">
         <v>237</v>
@@ -2390,21 +2403,21 @@
         <v>30</v>
       </c>
       <c r="B47" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C47" t="s">
         <v>238</v>
       </c>
       <c r="E47" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="B48" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="C48" t="s">
         <v>238</v>
@@ -2415,10 +2428,10 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="B49" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="C49" t="s">
         <v>238</v>
@@ -2432,10 +2445,10 @@
         <v>95</v>
       </c>
       <c r="B50" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E50" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -2452,7 +2465,7 @@
         <v>241</v>
       </c>
       <c r="E51" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -2471,10 +2484,10 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="B53" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>240</v>
@@ -2485,10 +2498,10 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="B54" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="C54" s="3" t="s">
         <v>240</v>
@@ -2511,15 +2524,15 @@
         <v>225</v>
       </c>
       <c r="E55" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="B56" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="C56" t="s">
         <v>240</v>
@@ -2530,10 +2543,10 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="B57" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="C57" t="s">
         <v>240</v>
@@ -2554,15 +2567,15 @@
       </c>
       <c r="D58" s="3"/>
       <c r="E58" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="B59" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="C59" s="3" t="s">
         <v>244</v>
@@ -2573,10 +2586,10 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="B60" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="C60" s="3" t="s">
         <v>244</v>
@@ -2590,13 +2603,13 @@
         <v>34</v>
       </c>
       <c r="B61" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="C61" t="s">
         <v>245</v>
       </c>
       <c r="E61" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -2604,13 +2617,13 @@
         <v>101</v>
       </c>
       <c r="B62" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="C62" t="s">
         <v>245</v>
       </c>
       <c r="E62" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -2621,22 +2634,22 @@
         <v>246</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="D63" s="3"/>
       <c r="E63" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="B64" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>204</v>
@@ -2644,13 +2657,13 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="B65" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="D65" s="2" t="s">
         <v>204</v>
@@ -2664,7 +2677,7 @@
         <v>247</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
@@ -2672,7 +2685,7 @@
         <v>37</v>
       </c>
       <c r="B67" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="C67" t="s">
         <v>203</v>
@@ -2689,7 +2702,7 @@
         <v>248</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="D68" t="s">
         <v>204</v>
@@ -2725,7 +2738,7 @@
         <v>41</v>
       </c>
       <c r="B71" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>204</v>
@@ -2736,7 +2749,7 @@
         <v>42</v>
       </c>
       <c r="B72" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>204</v>
@@ -2778,7 +2791,7 @@
         <v>45</v>
       </c>
       <c r="B75" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D75" t="s">
         <v>268</v>
@@ -2792,7 +2805,7 @@
         <v>46</v>
       </c>
       <c r="B76" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
@@ -2821,6 +2834,9 @@
       <c r="B79" t="s">
         <v>256</v>
       </c>
+      <c r="D79" t="s">
+        <v>204</v>
+      </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
@@ -2862,9 +2878,6 @@
       <c r="B83" t="s">
         <v>261</v>
       </c>
-      <c r="D83" t="s">
-        <v>204</v>
-      </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
@@ -3059,10 +3072,10 @@
         <v>72</v>
       </c>
       <c r="B102" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D102" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
@@ -3070,10 +3083,10 @@
         <v>73</v>
       </c>
       <c r="B103" t="s">
+        <v>391</v>
+      </c>
+      <c r="D103" t="s">
         <v>392</v>
-      </c>
-      <c r="D103" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
@@ -3081,13 +3094,13 @@
         <v>74</v>
       </c>
       <c r="B104" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C104" t="s">
         <v>258</v>
       </c>
       <c r="D104" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
@@ -3095,7 +3108,7 @@
         <v>75</v>
       </c>
       <c r="B105" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D105" t="s">
         <v>204</v>
@@ -3291,92 +3304,92 @@
         <v>90</v>
       </c>
       <c r="B122" t="s">
-        <v>314</v>
+        <v>482</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="B123" t="s">
-        <v>314</v>
+        <v>482</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="7" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="B124" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="D124" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="7" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="B125" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D125" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="7" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="B126" t="s">
+        <v>434</v>
+      </c>
+      <c r="D126" t="s">
         <v>437</v>
-      </c>
-      <c r="D126" t="s">
-        <v>440</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="7" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="B127" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="D127" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="7" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="B128" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="D128" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="7" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="B129" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="D129" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="7" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="B130" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="D130" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
@@ -3384,13 +3397,13 @@
         <v>91</v>
       </c>
       <c r="B131" t="s">
+        <v>314</v>
+      </c>
+      <c r="C131" t="s">
         <v>315</v>
       </c>
-      <c r="C131" t="s">
+      <c r="E131" t="s">
         <v>316</v>
-      </c>
-      <c r="E131" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
@@ -3398,21 +3411,21 @@
         <v>100</v>
       </c>
       <c r="B132" t="s">
+        <v>314</v>
+      </c>
+      <c r="C132" t="s">
         <v>315</v>
-      </c>
-      <c r="C132" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="B133" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="E133" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
@@ -3424,7 +3437,7 @@
       </c>
       <c r="C134" s="3"/>
       <c r="E134" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
@@ -3432,10 +3445,10 @@
         <v>103</v>
       </c>
       <c r="B135" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E135" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
@@ -3447,7 +3460,7 @@
       </c>
       <c r="C136" s="3"/>
       <c r="E136" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
@@ -3458,7 +3471,7 @@
         <v>294</v>
       </c>
       <c r="E137" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
@@ -3469,7 +3482,7 @@
         <v>304</v>
       </c>
       <c r="E138" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
@@ -3477,7 +3490,7 @@
         <v>108</v>
       </c>
       <c r="B139" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
@@ -3485,10 +3498,10 @@
         <v>109</v>
       </c>
       <c r="B140" t="s">
+        <v>318</v>
+      </c>
+      <c r="E140" t="s">
         <v>319</v>
-      </c>
-      <c r="E140" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
@@ -3496,7 +3509,7 @@
         <v>110</v>
       </c>
       <c r="B141" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
@@ -3504,7 +3517,7 @@
         <v>111</v>
       </c>
       <c r="B142" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
@@ -3512,10 +3525,10 @@
         <v>112</v>
       </c>
       <c r="B143" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="E143" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
@@ -3523,10 +3536,10 @@
         <v>113</v>
       </c>
       <c r="B144" t="s">
+        <v>323</v>
+      </c>
+      <c r="E144" t="s">
         <v>324</v>
-      </c>
-      <c r="E144" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
@@ -3534,10 +3547,10 @@
         <v>114</v>
       </c>
       <c r="B145" t="s">
+        <v>325</v>
+      </c>
+      <c r="C145" t="s">
         <v>326</v>
-      </c>
-      <c r="C145" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
@@ -3545,7 +3558,7 @@
         <v>115</v>
       </c>
       <c r="B146" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
@@ -3559,21 +3572,21 @@
         <v>199</v>
       </c>
       <c r="E147" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="B148" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C148" t="s">
         <v>199</v>
       </c>
       <c r="E148" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
@@ -3584,7 +3597,7 @@
         <v>215</v>
       </c>
       <c r="E149" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
@@ -3595,7 +3608,7 @@
         <v>299</v>
       </c>
       <c r="E150" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
@@ -3606,7 +3619,7 @@
         <v>294</v>
       </c>
       <c r="E151" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
@@ -3614,10 +3627,10 @@
         <v>120</v>
       </c>
       <c r="B152" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E152" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
@@ -3625,10 +3638,10 @@
         <v>121</v>
       </c>
       <c r="B153" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E153" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
@@ -3636,10 +3649,10 @@
         <v>122</v>
       </c>
       <c r="B154" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E154" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
@@ -3647,10 +3660,10 @@
         <v>123</v>
       </c>
       <c r="B155" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E155" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
@@ -3658,10 +3671,10 @@
         <v>124</v>
       </c>
       <c r="B156" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E156" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
@@ -3672,7 +3685,7 @@
         <v>305</v>
       </c>
       <c r="E157" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
@@ -3680,10 +3693,10 @@
         <v>126</v>
       </c>
       <c r="B158" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E158" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
@@ -3694,7 +3707,7 @@
         <v>301</v>
       </c>
       <c r="E159" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
@@ -3702,10 +3715,10 @@
         <v>128</v>
       </c>
       <c r="B160" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E160" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
@@ -3713,10 +3726,10 @@
         <v>129</v>
       </c>
       <c r="B161" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E161" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
@@ -3724,10 +3737,10 @@
         <v>130</v>
       </c>
       <c r="B162" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E162" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
@@ -3735,21 +3748,21 @@
         <v>131</v>
       </c>
       <c r="B163" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E163" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
+        <v>399</v>
+      </c>
+      <c r="B164" t="s">
         <v>400</v>
       </c>
-      <c r="B164" t="s">
-        <v>401</v>
-      </c>
       <c r="E164" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
@@ -3757,10 +3770,10 @@
         <v>132</v>
       </c>
       <c r="B165" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E165" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
@@ -3768,10 +3781,10 @@
         <v>133</v>
       </c>
       <c r="B166" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E166" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
@@ -3779,10 +3792,10 @@
         <v>134</v>
       </c>
       <c r="B167" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E167" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
@@ -3790,21 +3803,21 @@
         <v>135</v>
       </c>
       <c r="B168" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E168" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="B169" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="E169" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
@@ -3812,10 +3825,10 @@
         <v>136</v>
       </c>
       <c r="B170" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E170" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
@@ -3823,10 +3836,10 @@
         <v>137</v>
       </c>
       <c r="B171" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E171" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
@@ -3834,10 +3847,10 @@
         <v>138</v>
       </c>
       <c r="B172" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E172" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.25">
@@ -3845,10 +3858,10 @@
         <v>139</v>
       </c>
       <c r="B173" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E173" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.25">
@@ -3856,10 +3869,10 @@
         <v>140</v>
       </c>
       <c r="B174" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="E174" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.25">
@@ -3867,10 +3880,10 @@
         <v>141</v>
       </c>
       <c r="B175" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="E175" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.25">
@@ -3878,10 +3891,10 @@
         <v>142</v>
       </c>
       <c r="B176" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E176" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.25">
@@ -3889,10 +3902,10 @@
         <v>143</v>
       </c>
       <c r="B177" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="E177" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
@@ -3900,32 +3913,32 @@
         <v>144</v>
       </c>
       <c r="B178" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="E178" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="B179" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="E179" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="B180" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="E180" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.25">
@@ -3933,10 +3946,10 @@
         <v>145</v>
       </c>
       <c r="B181" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E181" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.25">
@@ -3947,7 +3960,7 @@
         <v>199</v>
       </c>
       <c r="E182" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.25">
@@ -3955,10 +3968,10 @@
         <v>147</v>
       </c>
       <c r="B183" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E183" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.25">
@@ -3966,10 +3979,10 @@
         <v>148</v>
       </c>
       <c r="B184" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="E184" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.25">
@@ -3980,7 +3993,7 @@
         <v>199</v>
       </c>
       <c r="E185" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.25">
@@ -3988,10 +4001,10 @@
         <v>150</v>
       </c>
       <c r="B186" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E186" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.25">
@@ -4002,7 +4015,7 @@
         <v>199</v>
       </c>
       <c r="E187" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.25">
@@ -4010,10 +4023,10 @@
         <v>152</v>
       </c>
       <c r="B188" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E188" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.25">
@@ -4024,7 +4037,7 @@
         <v>199</v>
       </c>
       <c r="E189" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.25">
@@ -4032,10 +4045,10 @@
         <v>154</v>
       </c>
       <c r="B190" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E190" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.25">
@@ -4046,7 +4059,7 @@
         <v>199</v>
       </c>
       <c r="E191" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.25">
@@ -4054,10 +4067,10 @@
         <v>156</v>
       </c>
       <c r="B192" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E192" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.25">
@@ -4068,7 +4081,7 @@
         <v>199</v>
       </c>
       <c r="E193" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.25">
@@ -4076,10 +4089,10 @@
         <v>158</v>
       </c>
       <c r="B194" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E194" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.25">
@@ -4090,7 +4103,7 @@
         <v>199</v>
       </c>
       <c r="E195" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.25">
@@ -4098,10 +4111,10 @@
         <v>160</v>
       </c>
       <c r="B196" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E196" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.25">
@@ -4112,7 +4125,7 @@
         <v>199</v>
       </c>
       <c r="E197" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.25">
@@ -4123,7 +4136,7 @@
         <v>199</v>
       </c>
       <c r="E198" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.25">
@@ -4131,10 +4144,10 @@
         <v>163</v>
       </c>
       <c r="B199" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E199" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.25">
@@ -4145,7 +4158,7 @@
         <v>199</v>
       </c>
       <c r="E200" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
@@ -4153,10 +4166,10 @@
         <v>165</v>
       </c>
       <c r="B201" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="E201" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.25">
@@ -4167,262 +4180,284 @@
         <v>199</v>
       </c>
       <c r="E202" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>403</v>
+        <v>483</v>
       </c>
       <c r="B203" t="s">
-        <v>402</v>
+        <v>485</v>
       </c>
       <c r="E203" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A204" t="s">
-        <v>441</v>
+      <c r="A204" s="8" t="s">
+        <v>484</v>
       </c>
       <c r="C204" t="s">
         <v>199</v>
       </c>
       <c r="E204" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A205" t="s">
-        <v>167</v>
+      <c r="A205" s="9" t="s">
+        <v>486</v>
       </c>
       <c r="B205" t="s">
-        <v>362</v>
+        <v>488</v>
       </c>
       <c r="E205" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A206" t="s">
-        <v>168</v>
+      <c r="A206" s="9" t="s">
+        <v>487</v>
       </c>
       <c r="C206" t="s">
         <v>199</v>
       </c>
       <c r="E206" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B207" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="E207" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C208" t="s">
         <v>199</v>
       </c>
       <c r="E208" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B209" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="E209" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C210" t="s">
         <v>199</v>
       </c>
       <c r="E210" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B211" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="E211" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C212" t="s">
         <v>199</v>
       </c>
       <c r="E212" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B213" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="E213" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C214" t="s">
         <v>199</v>
       </c>
       <c r="E214" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B215" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="E215" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C216" t="s">
         <v>199</v>
       </c>
       <c r="E216" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B217" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="E217" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C218" t="s">
         <v>199</v>
       </c>
       <c r="E218" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B219" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="E219" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C220" t="s">
         <v>199</v>
       </c>
       <c r="E220" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B221" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="E221" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>184</v>
-      </c>
-      <c r="B222" t="s">
-        <v>371</v>
+        <v>182</v>
+      </c>
+      <c r="C222" t="s">
+        <v>199</v>
       </c>
       <c r="E222" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B223" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="E223" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
+        <v>184</v>
+      </c>
+      <c r="B224" t="s">
+        <v>370</v>
+      </c>
+      <c r="E224" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A225" t="s">
+        <v>185</v>
+      </c>
+      <c r="B225" t="s">
+        <v>371</v>
+      </c>
+      <c r="E225" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A226" t="s">
         <v>186</v>
       </c>
-      <c r="B224" t="s">
+      <c r="B226" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A227" t="s">
+        <v>187</v>
+      </c>
+      <c r="B227" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A225" t="s">
-        <v>187</v>
-      </c>
-      <c r="B225" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A226" t="s">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A228" t="s">
         <v>188</v>
       </c>
-      <c r="B226" t="s">
-        <v>373</v>
+      <c r="B228" t="s">
+        <v>372</v>
       </c>
     </row>
   </sheetData>

</xml_diff>